<commit_message>
Made keyboard integration to send modes
</commit_message>
<xml_diff>
--- a/Rover Project Budget.xlsx
+++ b/Rover Project Budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Abdelrahman\University\Technical Teams\Torpedo\Rover_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423DDE54-339E-405D-9796-F0C5A78B6E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E91095B-80BD-4F6A-AD8A-A665A0FA79BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{54582110-3972-485A-B4F3-B6DCBCED3B6E}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -139,6 +139,15 @@
   </si>
   <si>
     <t>Capacitors</t>
+  </si>
+  <si>
+    <t>Pcb with components</t>
+  </si>
+  <si>
+    <t>regulators and stuff</t>
+  </si>
+  <si>
+    <t>acid</t>
   </si>
 </sst>
 </file>
@@ -531,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E6D0A54-75B1-4997-9DAB-FB578380BE60}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,8 +733,8 @@
         <v>22</v>
       </c>
       <c r="G11" cm="1">
-        <f t="array" ref="G11">SUM(C2:C12*D2:D12) +E20</f>
-        <v>275.8</v>
+        <f t="array" ref="G11">SUM(C2:C12*D2:D12) +E20+C21+C22+C23</f>
+        <v>379.40000000000003</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -750,7 +759,7 @@
       </c>
       <c r="G12">
         <f>G10-G11</f>
-        <v>224.2</v>
+        <v>120.59999999999997</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -797,6 +806,45 @@
       </c>
       <c r="E20">
         <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>68</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>15.6</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>